<commit_message>
Update sprint burndown chart
</commit_message>
<xml_diff>
--- a/docs/4_sprint_deliverables/Phase II/SprintBackLog - 2.xlsx
+++ b/docs/4_sprint_deliverables/Phase II/SprintBackLog - 2.xlsx
@@ -618,6 +618,118 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -644,118 +756,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -876,10 +876,10 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$29:$P$29</c:f>
+              <c:f>Sheet1!$K$29:$R$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>47.0</c:v>
                 </c:pt>
@@ -898,6 +898,12 @@
                 <c:pt idx="5">
                   <c:v>18.0</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -913,11 +919,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1652505840"/>
-        <c:axId val="1651989456"/>
+        <c:axId val="1674386192"/>
+        <c:axId val="1672936256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1652505840"/>
+        <c:axId val="1674386192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -953,7 +959,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1651989456"/>
+        <c:crossAx val="1672936256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -961,7 +967,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1651989456"/>
+        <c:axId val="1672936256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -991,7 +997,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1652505840"/>
+        <c:crossAx val="1674386192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1054,7 +1060,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1343,7 +1349,7 @@
   <dimension ref="B2:Z45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="83" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1445,19 +1451,19 @@
       </c>
     </row>
     <row r="3" spans="2:26" ht="62" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="51" t="s">
         <v>36</v>
       </c>
       <c r="G3" s="13" t="s">
@@ -1522,11 +1528,11 @@
       </c>
     </row>
     <row r="4" spans="2:26" ht="42" x14ac:dyDescent="0.15">
-      <c r="B4" s="29"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="26"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="52"/>
       <c r="G4" s="13" t="s">
         <v>38</v>
       </c>
@@ -1589,11 +1595,11 @@
       </c>
     </row>
     <row r="5" spans="2:26" ht="47" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="29"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="26"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="52"/>
       <c r="G5" s="13" t="s">
         <v>44</v>
       </c>
@@ -1656,11 +1662,11 @@
       </c>
     </row>
     <row r="6" spans="2:26" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="29"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="26"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="52"/>
       <c r="G6" s="13" t="s">
         <v>43</v>
       </c>
@@ -1723,850 +1729,850 @@
       </c>
     </row>
     <row r="7" spans="2:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="29"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="26"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="52"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
-      <c r="X7" s="16"/>
-      <c r="Y7" s="16"/>
-      <c r="Z7" s="16"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="54"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="54"/>
+      <c r="R7" s="54"/>
+      <c r="S7" s="54"/>
+      <c r="T7" s="54"/>
+      <c r="U7" s="54"/>
+      <c r="V7" s="54"/>
+      <c r="W7" s="54"/>
+      <c r="X7" s="54"/>
+      <c r="Y7" s="54"/>
+      <c r="Z7" s="54"/>
     </row>
     <row r="8" spans="2:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="29"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="26"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="52"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="17"/>
-      <c r="V8" s="17"/>
-      <c r="W8" s="17"/>
-      <c r="X8" s="17"/>
-      <c r="Y8" s="17"/>
-      <c r="Z8" s="17"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="55"/>
+      <c r="P8" s="55"/>
+      <c r="Q8" s="55"/>
+      <c r="R8" s="55"/>
+      <c r="S8" s="55"/>
+      <c r="T8" s="55"/>
+      <c r="U8" s="55"/>
+      <c r="V8" s="55"/>
+      <c r="W8" s="55"/>
+      <c r="X8" s="55"/>
+      <c r="Y8" s="55"/>
+      <c r="Z8" s="55"/>
     </row>
     <row r="9" spans="2:26" ht="147" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="29"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="27"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="53"/>
       <c r="G9" s="12"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="18"/>
-      <c r="W9" s="18"/>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="18"/>
-      <c r="Z9" s="18"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="56"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="56"/>
+      <c r="S9" s="56"/>
+      <c r="T9" s="56"/>
+      <c r="U9" s="56"/>
+      <c r="V9" s="56"/>
+      <c r="W9" s="56"/>
+      <c r="X9" s="56"/>
+      <c r="Y9" s="56"/>
+      <c r="Z9" s="56"/>
     </row>
     <row r="10" spans="2:26" ht="28" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="29"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="51" t="s">
+      <c r="B10" s="47"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="60" t="s">
+      <c r="F10" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="49" t="s">
+      <c r="G10" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="47" t="s">
+      <c r="H10" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="47" t="s">
+      <c r="I10" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="45">
+      <c r="J10" s="25">
         <v>3</v>
       </c>
-      <c r="K10" s="45">
+      <c r="K10" s="25">
         <v>3</v>
       </c>
-      <c r="L10" s="45">
-        <v>2</v>
-      </c>
-      <c r="M10" s="45">
+      <c r="L10" s="25">
+        <v>2</v>
+      </c>
+      <c r="M10" s="25">
         <v>1</v>
       </c>
-      <c r="N10" s="45">
-        <v>0</v>
-      </c>
-      <c r="O10" s="45">
-        <v>0</v>
-      </c>
-      <c r="P10" s="45">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="45">
-        <v>0</v>
-      </c>
-      <c r="R10" s="45">
-        <v>0</v>
-      </c>
-      <c r="S10" s="45">
-        <v>0</v>
-      </c>
-      <c r="T10" s="45">
-        <v>0</v>
-      </c>
-      <c r="U10" s="45">
-        <v>0</v>
-      </c>
-      <c r="V10" s="45">
-        <v>0</v>
-      </c>
-      <c r="W10" s="45">
-        <v>0</v>
-      </c>
-      <c r="X10" s="45">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="45">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="45">
+      <c r="N10" s="25">
+        <v>0</v>
+      </c>
+      <c r="O10" s="25">
+        <v>0</v>
+      </c>
+      <c r="P10" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="25">
+        <v>0</v>
+      </c>
+      <c r="R10" s="25">
+        <v>0</v>
+      </c>
+      <c r="S10" s="25">
+        <v>0</v>
+      </c>
+      <c r="T10" s="25">
+        <v>0</v>
+      </c>
+      <c r="U10" s="25">
+        <v>0</v>
+      </c>
+      <c r="V10" s="25">
+        <v>0</v>
+      </c>
+      <c r="W10" s="25">
+        <v>0</v>
+      </c>
+      <c r="X10" s="25">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="25">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="25">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:26" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="29"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="46"/>
-      <c r="S11" s="46"/>
-      <c r="T11" s="46"/>
-      <c r="U11" s="46"/>
-      <c r="V11" s="46"/>
-      <c r="W11" s="46"/>
-      <c r="X11" s="46"/>
-      <c r="Y11" s="46"/>
-      <c r="Z11" s="46"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="26"/>
+      <c r="U11" s="26"/>
+      <c r="V11" s="26"/>
+      <c r="W11" s="26"/>
+      <c r="X11" s="26"/>
+      <c r="Y11" s="26"/>
+      <c r="Z11" s="26"/>
     </row>
     <row r="12" spans="2:26" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="29"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="31" t="s">
+      <c r="B12" s="47"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="32" t="s">
+      <c r="H12" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="32" t="s">
+      <c r="I12" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="33">
+      <c r="J12" s="18">
         <v>3</v>
       </c>
-      <c r="K12" s="33">
+      <c r="K12" s="18">
         <v>3</v>
       </c>
-      <c r="L12" s="33">
+      <c r="L12" s="18">
         <v>3</v>
       </c>
-      <c r="M12" s="33">
+      <c r="M12" s="18">
         <v>3</v>
       </c>
-      <c r="N12" s="33">
+      <c r="N12" s="18">
         <v>3</v>
       </c>
-      <c r="O12" s="33">
+      <c r="O12" s="18">
         <v>3</v>
       </c>
-      <c r="P12" s="33">
-        <v>2</v>
-      </c>
-      <c r="Q12" s="33">
+      <c r="P12" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="18">
         <v>1</v>
       </c>
-      <c r="R12" s="33">
-        <v>0</v>
-      </c>
-      <c r="S12" s="33">
-        <v>0</v>
-      </c>
-      <c r="T12" s="33">
-        <v>0</v>
-      </c>
-      <c r="U12" s="33">
-        <v>0</v>
-      </c>
-      <c r="V12" s="33">
-        <v>0</v>
-      </c>
-      <c r="W12" s="33">
-        <v>0</v>
-      </c>
-      <c r="X12" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="33">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="33">
+      <c r="R12" s="18">
+        <v>0</v>
+      </c>
+      <c r="S12" s="18">
+        <v>0</v>
+      </c>
+      <c r="T12" s="18">
+        <v>0</v>
+      </c>
+      <c r="U12" s="18">
+        <v>0</v>
+      </c>
+      <c r="V12" s="18">
+        <v>0</v>
+      </c>
+      <c r="W12" s="18">
+        <v>0</v>
+      </c>
+      <c r="X12" s="18">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="18">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:26" ht="37" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="29"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="61"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="37"/>
       <c r="G13" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="34" t="s">
+      <c r="H13" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="32" t="s">
+      <c r="I13" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="J13" s="33">
-        <v>2</v>
-      </c>
-      <c r="K13" s="33">
-        <v>2</v>
-      </c>
-      <c r="L13" s="33">
-        <v>2</v>
-      </c>
-      <c r="M13" s="33">
-        <v>2</v>
-      </c>
-      <c r="N13" s="33">
-        <v>2</v>
-      </c>
-      <c r="O13" s="33">
-        <v>2</v>
-      </c>
-      <c r="P13" s="33">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="33">
+      <c r="J13" s="18">
+        <v>2</v>
+      </c>
+      <c r="K13" s="18">
+        <v>2</v>
+      </c>
+      <c r="L13" s="18">
+        <v>2</v>
+      </c>
+      <c r="M13" s="18">
+        <v>2</v>
+      </c>
+      <c r="N13" s="18">
+        <v>2</v>
+      </c>
+      <c r="O13" s="18">
+        <v>2</v>
+      </c>
+      <c r="P13" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="18">
         <v>1</v>
       </c>
-      <c r="R13" s="33">
-        <v>0</v>
-      </c>
-      <c r="S13" s="33">
-        <v>0</v>
-      </c>
-      <c r="T13" s="33">
-        <v>0</v>
-      </c>
-      <c r="U13" s="33">
-        <v>0</v>
-      </c>
-      <c r="V13" s="33">
-        <v>0</v>
-      </c>
-      <c r="W13" s="33">
-        <v>0</v>
-      </c>
-      <c r="X13" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="33">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="33">
+      <c r="R13" s="18">
+        <v>0</v>
+      </c>
+      <c r="S13" s="18">
+        <v>0</v>
+      </c>
+      <c r="T13" s="18">
+        <v>0</v>
+      </c>
+      <c r="U13" s="18">
+        <v>0</v>
+      </c>
+      <c r="V13" s="18">
+        <v>0</v>
+      </c>
+      <c r="W13" s="18">
+        <v>0</v>
+      </c>
+      <c r="X13" s="18">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="18">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:26" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="29"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="31" t="s">
+      <c r="B14" s="47"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="34" t="s">
+      <c r="H14" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="32" t="s">
+      <c r="I14" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="33">
-        <v>2</v>
-      </c>
-      <c r="K14" s="33">
-        <v>2</v>
-      </c>
-      <c r="L14" s="33">
-        <v>2</v>
-      </c>
-      <c r="M14" s="33">
-        <v>2</v>
-      </c>
-      <c r="N14" s="33">
-        <v>2</v>
-      </c>
-      <c r="O14" s="33">
-        <v>2</v>
-      </c>
-      <c r="P14" s="33">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="33">
+      <c r="J14" s="18">
+        <v>2</v>
+      </c>
+      <c r="K14" s="18">
+        <v>2</v>
+      </c>
+      <c r="L14" s="18">
+        <v>2</v>
+      </c>
+      <c r="M14" s="18">
+        <v>2</v>
+      </c>
+      <c r="N14" s="18">
+        <v>2</v>
+      </c>
+      <c r="O14" s="18">
+        <v>2</v>
+      </c>
+      <c r="P14" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="18">
         <v>1</v>
       </c>
-      <c r="R14" s="33">
-        <v>0</v>
-      </c>
-      <c r="S14" s="33">
-        <v>0</v>
-      </c>
-      <c r="T14" s="33">
-        <v>0</v>
-      </c>
-      <c r="U14" s="33">
-        <v>0</v>
-      </c>
-      <c r="V14" s="33">
-        <v>0</v>
-      </c>
-      <c r="W14" s="33">
-        <v>0</v>
-      </c>
-      <c r="X14" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="33">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="33">
+      <c r="R14" s="18">
+        <v>0</v>
+      </c>
+      <c r="S14" s="18">
+        <v>0</v>
+      </c>
+      <c r="T14" s="18">
+        <v>0</v>
+      </c>
+      <c r="U14" s="18">
+        <v>0</v>
+      </c>
+      <c r="V14" s="18">
+        <v>0</v>
+      </c>
+      <c r="W14" s="18">
+        <v>0</v>
+      </c>
+      <c r="X14" s="18">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="18">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:26" s="3" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="29"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="37"/>
-      <c r="S15" s="37"/>
-      <c r="T15" s="37"/>
-      <c r="U15" s="37"/>
-      <c r="V15" s="37"/>
-      <c r="W15" s="37"/>
-      <c r="X15" s="37"/>
-      <c r="Y15" s="37"/>
-      <c r="Z15" s="37"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
+      <c r="T15" s="22"/>
+      <c r="U15" s="22"/>
+      <c r="V15" s="22"/>
+      <c r="W15" s="22"/>
+      <c r="X15" s="22"/>
+      <c r="Y15" s="22"/>
+      <c r="Z15" s="22"/>
     </row>
     <row r="16" spans="2:26" ht="28" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="29"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="36"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="36"/>
-      <c r="R16" s="36"/>
-      <c r="S16" s="36"/>
-      <c r="T16" s="36"/>
-      <c r="U16" s="36"/>
-      <c r="V16" s="36"/>
-      <c r="W16" s="36"/>
-      <c r="X16" s="36"/>
-      <c r="Y16" s="36"/>
-      <c r="Z16" s="36"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="23"/>
+      <c r="W16" s="23"/>
+      <c r="X16" s="23"/>
+      <c r="Y16" s="23"/>
+      <c r="Z16" s="23"/>
     </row>
     <row r="17" spans="2:26" ht="147" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="29"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="38"/>
-      <c r="N17" s="38"/>
-      <c r="O17" s="38"/>
-      <c r="P17" s="38"/>
-      <c r="Q17" s="38"/>
-      <c r="R17" s="38"/>
-      <c r="S17" s="38"/>
-      <c r="T17" s="38"/>
-      <c r="U17" s="38"/>
-      <c r="V17" s="38"/>
-      <c r="W17" s="38"/>
-      <c r="X17" s="38"/>
-      <c r="Y17" s="38"/>
-      <c r="Z17" s="38"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
+      <c r="S17" s="24"/>
+      <c r="T17" s="24"/>
+      <c r="U17" s="24"/>
+      <c r="V17" s="24"/>
+      <c r="W17" s="24"/>
+      <c r="X17" s="24"/>
+      <c r="Y17" s="24"/>
+      <c r="Z17" s="24"/>
     </row>
     <row r="18" spans="2:26" x14ac:dyDescent="0.15">
-      <c r="B18" s="55"/>
-      <c r="C18" s="28" t="s">
+      <c r="B18" s="48"/>
+      <c r="C18" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="51" t="s">
+      <c r="E18" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="60" t="s">
+      <c r="F18" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="G18" s="49" t="s">
+      <c r="G18" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="H18" s="47" t="s">
+      <c r="H18" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="I18" s="47" t="s">
+      <c r="I18" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="45">
-        <v>2</v>
-      </c>
-      <c r="K18" s="45">
-        <v>2</v>
-      </c>
-      <c r="L18" s="45">
-        <v>2</v>
-      </c>
-      <c r="M18" s="45">
-        <v>2</v>
-      </c>
-      <c r="N18" s="45">
-        <v>2</v>
-      </c>
-      <c r="O18" s="45">
-        <v>2</v>
-      </c>
-      <c r="P18" s="45">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="45">
-        <v>0</v>
-      </c>
-      <c r="R18" s="45">
-        <v>0</v>
-      </c>
-      <c r="S18" s="45">
-        <v>0</v>
-      </c>
-      <c r="T18" s="45">
-        <v>0</v>
-      </c>
-      <c r="U18" s="45">
-        <v>0</v>
-      </c>
-      <c r="V18" s="45">
-        <v>0</v>
-      </c>
-      <c r="W18" s="45">
-        <v>0</v>
-      </c>
-      <c r="X18" s="45">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="45">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="45">
+      <c r="J18" s="25">
+        <v>2</v>
+      </c>
+      <c r="K18" s="25">
+        <v>2</v>
+      </c>
+      <c r="L18" s="25">
+        <v>2</v>
+      </c>
+      <c r="M18" s="25">
+        <v>2</v>
+      </c>
+      <c r="N18" s="25">
+        <v>2</v>
+      </c>
+      <c r="O18" s="25">
+        <v>2</v>
+      </c>
+      <c r="P18" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="25">
+        <v>0</v>
+      </c>
+      <c r="R18" s="25">
+        <v>0</v>
+      </c>
+      <c r="S18" s="25">
+        <v>0</v>
+      </c>
+      <c r="T18" s="25">
+        <v>0</v>
+      </c>
+      <c r="U18" s="25">
+        <v>0</v>
+      </c>
+      <c r="V18" s="25">
+        <v>0</v>
+      </c>
+      <c r="W18" s="25">
+        <v>0</v>
+      </c>
+      <c r="X18" s="25">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="25">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="25">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:26" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="55"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="46"/>
-      <c r="P19" s="46"/>
-      <c r="Q19" s="46"/>
-      <c r="R19" s="46"/>
-      <c r="S19" s="46"/>
-      <c r="T19" s="46"/>
-      <c r="U19" s="46"/>
-      <c r="V19" s="46"/>
-      <c r="W19" s="46"/>
-      <c r="X19" s="46"/>
-      <c r="Y19" s="46"/>
-      <c r="Z19" s="46"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="26"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="26"/>
+      <c r="T19" s="26"/>
+      <c r="U19" s="26"/>
+      <c r="V19" s="26"/>
+      <c r="W19" s="26"/>
+      <c r="X19" s="26"/>
+      <c r="Y19" s="26"/>
+      <c r="Z19" s="26"/>
     </row>
     <row r="20" spans="2:26" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="55"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="31" t="s">
+      <c r="B20" s="48"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="32" t="s">
+      <c r="H20" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="32" t="s">
+      <c r="I20" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="J20" s="33">
+      <c r="J20" s="18">
         <v>8</v>
       </c>
-      <c r="K20" s="33">
+      <c r="K20" s="18">
         <v>8</v>
       </c>
-      <c r="L20" s="33">
+      <c r="L20" s="18">
         <v>8</v>
       </c>
-      <c r="M20" s="33">
+      <c r="M20" s="18">
         <v>8</v>
       </c>
-      <c r="N20" s="33">
+      <c r="N20" s="18">
         <v>8</v>
       </c>
-      <c r="O20" s="33">
+      <c r="O20" s="18">
         <v>6</v>
       </c>
-      <c r="P20" s="33">
+      <c r="P20" s="18">
         <v>4</v>
       </c>
-      <c r="Q20" s="33">
-        <v>2</v>
-      </c>
-      <c r="R20" s="33">
-        <v>0</v>
-      </c>
-      <c r="S20" s="33">
-        <v>0</v>
-      </c>
-      <c r="T20" s="33">
-        <v>0</v>
-      </c>
-      <c r="U20" s="33">
-        <v>0</v>
-      </c>
-      <c r="V20" s="33">
-        <v>0</v>
-      </c>
-      <c r="W20" s="33">
-        <v>0</v>
-      </c>
-      <c r="X20" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="33">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="33">
+      <c r="Q20" s="18">
+        <v>2</v>
+      </c>
+      <c r="R20" s="18">
+        <v>0</v>
+      </c>
+      <c r="S20" s="18">
+        <v>0</v>
+      </c>
+      <c r="T20" s="18">
+        <v>0</v>
+      </c>
+      <c r="U20" s="18">
+        <v>0</v>
+      </c>
+      <c r="V20" s="18">
+        <v>0</v>
+      </c>
+      <c r="W20" s="18">
+        <v>0</v>
+      </c>
+      <c r="X20" s="18">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="18">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:26" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="55"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="61"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="37"/>
       <c r="G21" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="H21" s="34" t="s">
+      <c r="H21" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="I21" s="32" t="s">
+      <c r="I21" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="J21" s="33">
+      <c r="J21" s="18">
         <v>5</v>
       </c>
-      <c r="K21" s="33">
+      <c r="K21" s="18">
         <v>5</v>
       </c>
-      <c r="L21" s="33">
+      <c r="L21" s="18">
         <v>4</v>
       </c>
-      <c r="M21" s="33">
-        <v>2</v>
-      </c>
-      <c r="N21" s="33">
+      <c r="M21" s="18">
+        <v>2</v>
+      </c>
+      <c r="N21" s="18">
         <v>1</v>
       </c>
-      <c r="O21" s="33">
-        <v>0</v>
-      </c>
-      <c r="P21" s="33">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="33">
-        <v>0</v>
-      </c>
-      <c r="R21" s="33">
-        <v>0</v>
-      </c>
-      <c r="S21" s="33">
-        <v>0</v>
-      </c>
-      <c r="T21" s="33">
-        <v>0</v>
-      </c>
-      <c r="U21" s="33">
-        <v>0</v>
-      </c>
-      <c r="V21" s="33">
-        <v>0</v>
-      </c>
-      <c r="W21" s="33">
-        <v>0</v>
-      </c>
-      <c r="X21" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="33">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="33"/>
+      <c r="O21" s="18">
+        <v>0</v>
+      </c>
+      <c r="P21" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="18">
+        <v>0</v>
+      </c>
+      <c r="R21" s="18">
+        <v>0</v>
+      </c>
+      <c r="S21" s="18">
+        <v>0</v>
+      </c>
+      <c r="T21" s="18">
+        <v>0</v>
+      </c>
+      <c r="U21" s="18">
+        <v>0</v>
+      </c>
+      <c r="V21" s="18">
+        <v>0</v>
+      </c>
+      <c r="W21" s="18">
+        <v>0</v>
+      </c>
+      <c r="X21" s="18">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="18">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="18"/>
     </row>
     <row r="22" spans="2:26" ht="38" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="55"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="31" t="s">
+      <c r="B22" s="48"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="H22" s="34" t="s">
+      <c r="H22" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I22" s="32" t="s">
+      <c r="I22" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="J22" s="33">
-        <v>2</v>
-      </c>
-      <c r="K22" s="33">
-        <v>2</v>
-      </c>
-      <c r="L22" s="33">
-        <v>2</v>
-      </c>
-      <c r="M22" s="33">
-        <v>2</v>
-      </c>
-      <c r="N22" s="33">
-        <v>2</v>
-      </c>
-      <c r="O22" s="33">
-        <v>2</v>
-      </c>
-      <c r="P22" s="33">
-        <v>2</v>
-      </c>
-      <c r="Q22" s="33">
+      <c r="J22" s="18">
+        <v>2</v>
+      </c>
+      <c r="K22" s="18">
+        <v>2</v>
+      </c>
+      <c r="L22" s="18">
+        <v>2</v>
+      </c>
+      <c r="M22" s="18">
+        <v>2</v>
+      </c>
+      <c r="N22" s="18">
+        <v>2</v>
+      </c>
+      <c r="O22" s="18">
+        <v>2</v>
+      </c>
+      <c r="P22" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q22" s="18">
         <v>1</v>
       </c>
-      <c r="R22" s="33">
-        <v>0</v>
-      </c>
-      <c r="S22" s="33">
-        <v>0</v>
-      </c>
-      <c r="T22" s="33">
-        <v>0</v>
-      </c>
-      <c r="U22" s="33">
-        <v>0</v>
-      </c>
-      <c r="V22" s="33">
-        <v>0</v>
-      </c>
-      <c r="W22" s="33">
-        <v>0</v>
-      </c>
-      <c r="X22" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="33">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="33">
+      <c r="R22" s="18">
+        <v>0</v>
+      </c>
+      <c r="S22" s="18">
+        <v>0</v>
+      </c>
+      <c r="T22" s="18">
+        <v>0</v>
+      </c>
+      <c r="U22" s="18">
+        <v>0</v>
+      </c>
+      <c r="V22" s="18">
+        <v>0</v>
+      </c>
+      <c r="W22" s="18">
+        <v>0</v>
+      </c>
+      <c r="X22" s="18">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="18">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:26" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="55"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="37"/>
-      <c r="N23" s="37"/>
-      <c r="O23" s="37"/>
-      <c r="P23" s="37"/>
-      <c r="Q23" s="37"/>
-      <c r="R23" s="37"/>
-      <c r="S23" s="37"/>
-      <c r="T23" s="37"/>
-      <c r="U23" s="37"/>
-      <c r="V23" s="37"/>
-      <c r="W23" s="37"/>
-      <c r="X23" s="37"/>
-      <c r="Y23" s="37"/>
-      <c r="Z23" s="37"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="22"/>
+      <c r="S23" s="22"/>
+      <c r="T23" s="22"/>
+      <c r="U23" s="22"/>
+      <c r="V23" s="22"/>
+      <c r="W23" s="22"/>
+      <c r="X23" s="22"/>
+      <c r="Y23" s="22"/>
+      <c r="Z23" s="22"/>
     </row>
     <row r="24" spans="2:26" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="55"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="36"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="36"/>
-      <c r="Q24" s="36"/>
-      <c r="R24" s="36"/>
-      <c r="S24" s="36"/>
-      <c r="T24" s="36"/>
-      <c r="U24" s="36"/>
-      <c r="V24" s="36"/>
-      <c r="W24" s="36"/>
-      <c r="X24" s="36"/>
-      <c r="Y24" s="36"/>
-      <c r="Z24" s="36"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
+      <c r="U24" s="23"/>
+      <c r="V24" s="23"/>
+      <c r="W24" s="23"/>
+      <c r="X24" s="23"/>
+      <c r="Y24" s="23"/>
+      <c r="Z24" s="23"/>
     </row>
     <row r="25" spans="2:26" ht="158" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="56"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="38"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="38"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="38"/>
-      <c r="U25" s="38"/>
-      <c r="V25" s="38"/>
-      <c r="W25" s="38"/>
-      <c r="X25" s="38"/>
-      <c r="Y25" s="38"/>
-      <c r="Z25" s="38"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24"/>
+      <c r="S25" s="24"/>
+      <c r="T25" s="24"/>
+      <c r="U25" s="24"/>
+      <c r="V25" s="24"/>
+      <c r="W25" s="24"/>
+      <c r="X25" s="24"/>
+      <c r="Y25" s="24"/>
+      <c r="Z25" s="24"/>
     </row>
     <row r="26" spans="2:26" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C26" s="54"/>
+      <c r="C26" s="21"/>
     </row>
     <row r="27" spans="2:26" ht="13" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="28" spans="2:26" ht="13" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2697,6 +2703,90 @@
     </row>
   </sheetData>
   <mergeCells count="108">
+    <mergeCell ref="Z7:Z9"/>
+    <mergeCell ref="S7:S9"/>
+    <mergeCell ref="T7:T9"/>
+    <mergeCell ref="U7:U9"/>
+    <mergeCell ref="V7:V9"/>
+    <mergeCell ref="W7:W9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="O7:O9"/>
+    <mergeCell ref="P7:P9"/>
+    <mergeCell ref="Q7:Q9"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="X7:X9"/>
+    <mergeCell ref="Y7:Y9"/>
+    <mergeCell ref="Q10:Q11"/>
+    <mergeCell ref="P10:P11"/>
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="Z15:Z17"/>
+    <mergeCell ref="Y15:Y17"/>
+    <mergeCell ref="X15:X17"/>
+    <mergeCell ref="W15:W17"/>
+    <mergeCell ref="V15:V17"/>
+    <mergeCell ref="U15:U17"/>
+    <mergeCell ref="T15:T17"/>
+    <mergeCell ref="S15:S17"/>
+    <mergeCell ref="R15:R17"/>
+    <mergeCell ref="Q15:Q17"/>
+    <mergeCell ref="P15:P17"/>
+    <mergeCell ref="O15:O17"/>
+    <mergeCell ref="Z10:Z11"/>
+    <mergeCell ref="Y10:Y11"/>
+    <mergeCell ref="X10:X11"/>
+    <mergeCell ref="W10:W11"/>
+    <mergeCell ref="V10:V11"/>
+    <mergeCell ref="U10:U11"/>
+    <mergeCell ref="T10:T11"/>
+    <mergeCell ref="S10:S11"/>
+    <mergeCell ref="R10:R11"/>
+    <mergeCell ref="C3:C17"/>
+    <mergeCell ref="D3:D17"/>
+    <mergeCell ref="F10:F17"/>
+    <mergeCell ref="B3:B25"/>
+    <mergeCell ref="D18:D25"/>
+    <mergeCell ref="C18:C25"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="N15:N17"/>
+    <mergeCell ref="M15:M17"/>
+    <mergeCell ref="L15:L17"/>
+    <mergeCell ref="F3:F9"/>
+    <mergeCell ref="E3:E9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="E18:E25"/>
+    <mergeCell ref="F18:F25"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="E10:E17"/>
+    <mergeCell ref="W18:W19"/>
+    <mergeCell ref="X18:X19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="S18:S19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
     <mergeCell ref="V23:V25"/>
     <mergeCell ref="W23:W25"/>
     <mergeCell ref="X23:X25"/>
@@ -2721,90 +2811,6 @@
     <mergeCell ref="T18:T19"/>
     <mergeCell ref="U18:U19"/>
     <mergeCell ref="V18:V19"/>
-    <mergeCell ref="W18:W19"/>
-    <mergeCell ref="X18:X19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="Q18:Q19"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="S18:S19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="E18:E25"/>
-    <mergeCell ref="F18:F25"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="E10:E17"/>
-    <mergeCell ref="C3:C17"/>
-    <mergeCell ref="D3:D17"/>
-    <mergeCell ref="F10:F17"/>
-    <mergeCell ref="B3:B25"/>
-    <mergeCell ref="D18:D25"/>
-    <mergeCell ref="C18:C25"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K15:K17"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="Z10:Z11"/>
-    <mergeCell ref="Y10:Y11"/>
-    <mergeCell ref="X10:X11"/>
-    <mergeCell ref="W10:W11"/>
-    <mergeCell ref="V10:V11"/>
-    <mergeCell ref="U10:U11"/>
-    <mergeCell ref="T10:T11"/>
-    <mergeCell ref="S10:S11"/>
-    <mergeCell ref="R10:R11"/>
-    <mergeCell ref="Q10:Q11"/>
-    <mergeCell ref="P10:P11"/>
-    <mergeCell ref="O10:O11"/>
-    <mergeCell ref="Z15:Z17"/>
-    <mergeCell ref="Y15:Y17"/>
-    <mergeCell ref="X15:X17"/>
-    <mergeCell ref="W15:W17"/>
-    <mergeCell ref="V15:V17"/>
-    <mergeCell ref="U15:U17"/>
-    <mergeCell ref="T15:T17"/>
-    <mergeCell ref="S15:S17"/>
-    <mergeCell ref="R15:R17"/>
-    <mergeCell ref="Q15:Q17"/>
-    <mergeCell ref="P15:P17"/>
-    <mergeCell ref="O15:O17"/>
-    <mergeCell ref="N15:N17"/>
-    <mergeCell ref="M15:M17"/>
-    <mergeCell ref="L15:L17"/>
-    <mergeCell ref="F3:F9"/>
-    <mergeCell ref="E3:E9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="O7:O9"/>
-    <mergeCell ref="P7:P9"/>
-    <mergeCell ref="Q7:Q9"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="X7:X9"/>
-    <mergeCell ref="Y7:Y9"/>
-    <mergeCell ref="Z7:Z9"/>
-    <mergeCell ref="S7:S9"/>
-    <mergeCell ref="T7:T9"/>
-    <mergeCell ref="U7:U9"/>
-    <mergeCell ref="V7:V9"/>
-    <mergeCell ref="W7:W9"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>